<commit_message>
calculating percent of populations represented in CNA areas, by guild, and plotting results
</commit_message>
<xml_diff>
--- a/outputs/summary_pct_pop_guild_carbon_90pct_RAN.xlsx
+++ b/outputs/summary_pct_pop_guild_carbon_90pct_RAN.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raenb\Documents\GitHub\es_birds_usa\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FED17483-DEBC-40ED-A734-C0D99F4E2005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614022C2-BFBB-469F-92C3-29145ABE07AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15600"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_pct_pop_guild_carbon_90" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>more90</t>
   </si>
@@ -51,11 +51,14 @@
   <si>
     <t>generalist</t>
   </si>
+  <si>
+    <t>n</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -534,10 +537,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -893,114 +895,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="3" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1">
         <v>1.7543859649122799E-2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="1">
         <v>0.157894736842105</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="1">
         <v>0.33333333333333298</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
+        <v>184</v>
+      </c>
+      <c r="C3" s="1">
         <v>3.2608695652173898E-2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="1">
         <v>0.25</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="1">
         <v>0.77173913043478204</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="1">
         <v>0.17391304347826</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="1">
         <v>1.7543859649122799E-2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="1">
         <v>5.2631578947368397E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
+        <v>120</v>
+      </c>
+      <c r="C6" s="1">
         <v>8.4033613445378096E-3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="1">
         <v>1.6806722689075598E-2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="1">
         <v>0.17647058823529399</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1">
         <v>0</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="1">
         <v>0.21052631578947301</v>
       </c>
     </row>
@@ -1010,6 +1033,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D2564070661E224EB529D764830DFF91" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fc2897e26550864c72d1388ce1418d20">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="206e467f-b0cb-4c8c-912a-bab5a509c489" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8d74fc544fda12cc11568f996aa1415" ns3:_="">
     <xsd:import namespace="206e467f-b0cb-4c8c-912a-bab5a509c489"/>
@@ -1161,15 +1193,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1179,6 +1202,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46997B7A-022A-4315-8D6E-28761855840C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F81C2D46-4EE9-4731-AB08-63145AAAC406}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1192,14 +1223,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46997B7A-022A-4315-8D6E-28761855840C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>